<commit_message>
finalised plasmid ont protocol
</commit_message>
<xml_diff>
--- a/templates/02-ont-plasmid.xlsx
+++ b/templates/02-ont-plasmid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloas/code/opentrons/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4116326-6808-2544-9BFC-FF8917815512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FF14F4-26B3-1D47-803D-E31BC3D33F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="1360" windowWidth="27920" windowHeight="15940" activeTab="2" xr2:uid="{0E74BB9A-F8B8-AA47-B7C7-EA2C2417D685}"/>
+    <workbookView xWindow="1700" yWindow="1360" windowWidth="27920" windowHeight="15940" xr2:uid="{0E74BB9A-F8B8-AA47-B7C7-EA2C2417D685}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="348">
   <si>
     <t>Plasmid sequencing ONT at BCL - Opentrons template</t>
   </si>
@@ -1042,9 +1042,6 @@
     <t>sample 15</t>
   </si>
   <si>
-    <t>dest well2</t>
-  </si>
-  <si>
     <t>This template is used to prepare the data for protocols/ont-plasmid.py</t>
   </si>
   <si>
@@ -1094,6 +1091,18 @@
   </si>
   <si>
     <t>sample 22</t>
+  </si>
+  <si>
+    <t>barcode well</t>
+  </si>
+  <si>
+    <t>dest well</t>
+  </si>
+  <si>
+    <t>final library</t>
+  </si>
+  <si>
+    <t>tuberack B1</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1260,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1301,24 +1313,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59494247-6707-4A4B-A68E-97E8FDDD4AF4}" name="Table1" displayName="Table1" ref="B8:J104" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="B8:J104" xr:uid="{59494247-6707-4A4B-A68E-97E8FDDD4AF4}"/>
-  <tableColumns count="9">
-    <tableColumn id="8" xr3:uid="{FA78698F-F611-D543-B141-D777144BECEE}" name="source well" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59494247-6707-4A4B-A68E-97E8FDDD4AF4}" name="Table1" displayName="Table1" ref="B8:K104" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="B8:K104" xr:uid="{59494247-6707-4A4B-A68E-97E8FDDD4AF4}"/>
+  <tableColumns count="10">
+    <tableColumn id="8" xr3:uid="{FA78698F-F611-D543-B141-D777144BECEE}" name="source well" dataDxfId="5"/>
     <tableColumn id="1" xr3:uid="{91DE4E1A-6DA9-5D41-9DB5-21149FC9505F}" name="sample name"/>
     <tableColumn id="7" xr3:uid="{E7F73DE6-44A2-FD49-95BC-9E263FB79FB0}" name="barcode"/>
     <tableColumn id="2" xr3:uid="{D3E7E880-2BC6-B94A-AFA4-408237577810}" name="plasmid size"/>
     <tableColumn id="3" xr3:uid="{AF07D2D6-012E-8643-901A-5055CCEAF026}" name="ng/ul"/>
-    <tableColumn id="4" xr3:uid="{80D148B5-CECA-CA44-B1DD-F9E1A8DAA6A0}" name="fmol/ul" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{80D148B5-CECA-CA44-B1DD-F9E1A8DAA6A0}" name="fmol/ul" dataDxfId="4">
       <calculatedColumnFormula>F9/((E9*617.96)+36.04) * 1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{6A4DD60B-B1AB-FF44-9E4F-4697D7C0CC9E}" name="ul plasmid" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{6A4DD60B-B1AB-FF44-9E4F-4697D7C0CC9E}" name="ul plasmid" dataDxfId="3">
       <calculatedColumnFormula array="1">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;4.5,4.5,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{53D08A06-9EBD-1143-A0BC-3E9BC0C89175}" name="ul water to 4.5" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{53D08A06-9EBD-1143-A0BC-3E9BC0C89175}" name="ul water to 4.5" dataDxfId="2">
       <calculatedColumnFormula>IF(Table1[[#This Row],[ul plasmid]]=0,0,4.5-Table1[[#This Row],[ul plasmid]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0EE7AD1A-A1CC-364C-B346-C43B6AB6BFEF}" name="dest well2" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{0EE7AD1A-A1CC-364C-B346-C43B6AB6BFEF}" name="dest well" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{DDAE90F6-C57C-A64E-B7AF-286C3EB0FE38}" name="barcode well" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1633,10 +1648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842AFD07-9B34-384A-83A8-BAD898DE59C4}">
-  <dimension ref="B1:P105"/>
+  <dimension ref="B1:R105"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1648,33 +1663,36 @@
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" customWidth="1"/>
     <col min="15" max="15" width="12.5" customWidth="1"/>
     <col min="16" max="16" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="M4" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1685,7 +1703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -1695,34 +1713,34 @@
       <c r="J6">
         <v>0.5</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
+        <v>329</v>
+      </c>
+      <c r="N6" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="P6" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
         <v>331</v>
       </c>
-      <c r="O6" t="s">
-        <v>314</v>
-      </c>
-      <c r="P6" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="L7" t="s">
-        <v>332</v>
-      </c>
-      <c r="M7" s="12">
+      <c r="N7" s="12">
         <v>4</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>317</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>313</v>
       </c>
@@ -1748,22 +1766,25 @@
         <v>7</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="L8" t="s">
+        <v>345</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="M8" t="s">
         <v>324</v>
       </c>
-      <c r="M8" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="N8" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q8" t="s">
         <v>320</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>120</v>
       </c>
@@ -1794,19 +1815,23 @@
       <c r="J9" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="L9" t="s">
-        <v>337</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="K9" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>A01</v>
+      </c>
+      <c r="M9" t="s">
+        <v>336</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D10" t="s">
         <v>218</v>
@@ -1832,19 +1857,23 @@
       <c r="J10" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="L10" t="s">
-        <v>336</v>
-      </c>
-      <c r="M10" s="12" t="s">
+      <c r="K10" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>B01</v>
+      </c>
+      <c r="M10" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N10" s="12" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D11" t="s">
         <v>219</v>
@@ -1870,13 +1899,17 @@
       <c r="J11" s="9" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="K11" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>C01</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D12" t="s">
         <v>220</v>
@@ -1902,13 +1935,23 @@
       <c r="J12" s="9" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="K12" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>D01</v>
+      </c>
+      <c r="M12" t="s">
+        <v>346</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D13" t="s">
         <v>221</v>
@@ -1934,14 +1977,18 @@
       <c r="J13" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="M13" s="11"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="K13" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>E01</v>
+      </c>
+      <c r="N13" s="11"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D14" t="s">
         <v>222</v>
@@ -1967,13 +2014,17 @@
       <c r="J14" s="9" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="K14" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>F01</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C15" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D15" t="s">
         <v>223</v>
@@ -1999,13 +2050,17 @@
       <c r="J15" s="9" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="K15" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>G01</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D16" t="s">
         <v>224</v>
@@ -2031,8 +2086,12 @@
       <c r="J16" s="9" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>H01</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="G17" s="2">
         <f>F17/((E17*617.96)+36.04) * 1000000</f>
@@ -2049,8 +2108,12 @@
       <c r="J17" s="9" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="G18" s="2">
         <f>F18/((E18*617.96)+36.04) * 1000000</f>
@@ -2067,8 +2130,12 @@
       <c r="J18" s="9" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="G19" s="2">
         <f>F19/((E19*617.96)+36.04) * 1000000</f>
@@ -2085,8 +2152,12 @@
       <c r="J19" s="9" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="G20" s="2">
         <f>F20/((E20*617.96)+36.04) * 1000000</f>
@@ -2103,8 +2174,12 @@
       <c r="J20" s="9" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="G21" s="2">
         <f>F21/((E21*617.96)+36.04) * 1000000</f>
@@ -2121,8 +2196,12 @@
       <c r="J21" s="9" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="G22" s="2">
         <f>F22/((E22*617.96)+36.04) * 1000000</f>
@@ -2139,8 +2218,12 @@
       <c r="J22" s="9" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="G23" s="2">
         <f>F23/((E23*617.96)+36.04) * 1000000</f>
@@ -2157,8 +2240,12 @@
       <c r="J23" s="9" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="G24" s="2">
         <f t="shared" ref="G24" si="0">F24/((E24*617.96)+36.04) * 1000000</f>
@@ -2175,8 +2262,12 @@
       <c r="J24" s="9" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>120</v>
       </c>
@@ -2207,8 +2298,12 @@
       <c r="J25" s="9" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>A02</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>121</v>
       </c>
@@ -2239,8 +2334,12 @@
       <c r="J26" s="9" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>B02</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>122</v>
       </c>
@@ -2271,8 +2370,12 @@
       <c r="J27" s="9" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>C02</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>123</v>
       </c>
@@ -2303,8 +2406,12 @@
       <c r="J28" s="9" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>D02</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>124</v>
       </c>
@@ -2335,8 +2442,12 @@
       <c r="J29" s="9" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>E02</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>125</v>
       </c>
@@ -2367,8 +2478,12 @@
       <c r="J30" s="9" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K30" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>F02</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>126</v>
       </c>
@@ -2399,8 +2514,12 @@
       <c r="J31" s="9" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>G02</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>127</v>
       </c>
@@ -2431,8 +2550,12 @@
       <c r="J32" s="9" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v>H02</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="G33" s="2">
         <f>F33/((E33*617.96)+36.04) * 1000000</f>
@@ -2449,8 +2572,12 @@
       <c r="J33" s="9" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="G34" s="2">
         <f>F34/((E34*617.96)+36.04) * 1000000</f>
@@ -2467,8 +2594,12 @@
       <c r="J34" s="9" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
       <c r="G35" s="2">
         <f>F35/((E35*617.96)+36.04) * 1000000</f>
@@ -2485,8 +2616,12 @@
       <c r="J35" s="9" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="G36" s="2">
         <f>F36/((E36*617.96)+36.04) * 1000000</f>
@@ -2503,8 +2638,12 @@
       <c r="J36" s="9" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="G37" s="2">
         <f>F37/((E37*617.96)+36.04) * 1000000</f>
@@ -2521,8 +2660,12 @@
       <c r="J37" s="9" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K37" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="G38" s="2">
         <f>F38/((E38*617.96)+36.04) * 1000000</f>
@@ -2539,8 +2682,12 @@
       <c r="J38" s="9" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="G39" s="2">
         <f t="shared" ref="G39:G57" si="1">F39/((E39*617.96)+36.04) * 1000000</f>
@@ -2557,8 +2704,12 @@
       <c r="J39" s="9" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K39" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
       <c r="G40" s="2">
         <f t="shared" si="1"/>
@@ -2575,8 +2726,12 @@
       <c r="J40" s="9" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K40" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="G41" s="2">
         <f t="shared" si="1"/>
@@ -2593,8 +2748,12 @@
       <c r="J41" s="9" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B42" s="2"/>
       <c r="G42" s="2">
         <f t="shared" si="1"/>
@@ -2611,8 +2770,12 @@
       <c r="J42" s="9" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
       <c r="G43" s="2">
         <f t="shared" si="1"/>
@@ -2629,8 +2792,12 @@
       <c r="J43" s="9" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K43" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B44" s="2"/>
       <c r="G44" s="2">
         <f t="shared" si="1"/>
@@ -2647,8 +2814,12 @@
       <c r="J44" s="9" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K44" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="2"/>
       <c r="G45" s="2">
         <f t="shared" si="1"/>
@@ -2665,8 +2836,12 @@
       <c r="J45" s="9" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K45" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
       <c r="G46" s="2">
         <f t="shared" si="1"/>
@@ -2683,8 +2858,12 @@
       <c r="J46" s="9" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K46" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
       <c r="G47" s="2">
         <f t="shared" si="1"/>
@@ -2701,8 +2880,12 @@
       <c r="J47" s="9" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K47" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="2"/>
       <c r="G48" s="2">
         <f t="shared" si="1"/>
@@ -2719,8 +2902,12 @@
       <c r="J48" s="9" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K48" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B49" s="2"/>
       <c r="G49" s="2">
         <f t="shared" si="1"/>
@@ -2737,8 +2924,12 @@
       <c r="J49" s="9" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K49" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B50" s="2"/>
       <c r="G50" s="2">
         <f t="shared" si="1"/>
@@ -2755,8 +2946,12 @@
       <c r="J50" s="9" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K50" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B51" s="2"/>
       <c r="G51" s="2">
         <f t="shared" si="1"/>
@@ -2773,8 +2968,12 @@
       <c r="J51" s="9" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K51" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="G52" s="2">
         <f t="shared" si="1"/>
@@ -2791,8 +2990,12 @@
       <c r="J52" s="9" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K52" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="G53" s="2">
         <f t="shared" si="1"/>
@@ -2809,8 +3012,12 @@
       <c r="J53" s="9" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K53" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="G54" s="2">
         <f t="shared" si="1"/>
@@ -2827,8 +3034,12 @@
       <c r="J54" s="9" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K54" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="G55" s="2">
         <f t="shared" si="1"/>
@@ -2845,8 +3056,12 @@
       <c r="J55" s="9" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K55" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="G56" s="2">
         <f t="shared" si="1"/>
@@ -2863,8 +3078,12 @@
       <c r="J56" s="9" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K56" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="G57" s="2">
         <f t="shared" si="1"/>
@@ -2881,8 +3100,12 @@
       <c r="J57" s="9" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K57" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="G58" s="2">
         <f t="shared" ref="G58:G89" si="2">F58/((E58*617.96)+36.04) * 1000000</f>
@@ -2899,8 +3122,12 @@
       <c r="J58" s="9" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K58" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="G59" s="2">
         <f t="shared" si="2"/>
@@ -2917,8 +3144,12 @@
       <c r="J59" s="9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K59" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="G60" s="2">
         <f t="shared" si="2"/>
@@ -2935,8 +3166,12 @@
       <c r="J60" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K60" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="G61" s="2">
         <f t="shared" si="2"/>
@@ -2953,8 +3188,12 @@
       <c r="J61" s="9" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K61" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="G62" s="2">
         <f t="shared" si="2"/>
@@ -2971,8 +3210,12 @@
       <c r="J62" s="9" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K62" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="G63" s="2">
         <f t="shared" si="2"/>
@@ -2989,8 +3232,12 @@
       <c r="J63" s="9" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K63" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="G64" s="2">
         <f t="shared" si="2"/>
@@ -3007,8 +3254,12 @@
       <c r="J64" s="9" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K64" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B65" s="2"/>
       <c r="G65" s="2">
         <f t="shared" si="2"/>
@@ -3025,8 +3276,12 @@
       <c r="J65" s="9" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K65" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B66" s="2"/>
       <c r="G66" s="2">
         <f t="shared" si="2"/>
@@ -3043,8 +3298,12 @@
       <c r="J66" s="9" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K66" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B67" s="2"/>
       <c r="G67" s="2">
         <f t="shared" si="2"/>
@@ -3061,8 +3320,12 @@
       <c r="J67" s="9" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K67" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B68" s="2"/>
       <c r="G68" s="2">
         <f t="shared" si="2"/>
@@ -3079,8 +3342,12 @@
       <c r="J68" s="9" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K68" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B69" s="2"/>
       <c r="G69" s="2">
         <f t="shared" si="2"/>
@@ -3097,8 +3364,12 @@
       <c r="J69" s="9" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K69" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B70" s="2"/>
       <c r="G70" s="2">
         <f t="shared" si="2"/>
@@ -3115,8 +3386,12 @@
       <c r="J70" s="9" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K70" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B71" s="2"/>
       <c r="G71" s="2">
         <f t="shared" si="2"/>
@@ -3133,8 +3408,12 @@
       <c r="J71" s="9" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K71" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B72" s="2"/>
       <c r="G72" s="2">
         <f t="shared" si="2"/>
@@ -3151,8 +3430,12 @@
       <c r="J72" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K72" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B73" s="2"/>
       <c r="G73" s="2">
         <f t="shared" si="2"/>
@@ -3169,8 +3452,12 @@
       <c r="J73" s="9" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K73" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B74" s="2"/>
       <c r="G74" s="2">
         <f t="shared" si="2"/>
@@ -3187,8 +3474,12 @@
       <c r="J74" s="9" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K74" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B75" s="2"/>
       <c r="G75" s="2">
         <f t="shared" si="2"/>
@@ -3205,8 +3496,12 @@
       <c r="J75" s="9" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K75" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B76" s="2"/>
       <c r="G76" s="2">
         <f t="shared" si="2"/>
@@ -3223,8 +3518,12 @@
       <c r="J76" s="9" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K76" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B77" s="2"/>
       <c r="G77" s="2">
         <f t="shared" si="2"/>
@@ -3241,8 +3540,12 @@
       <c r="J77" s="9" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K77" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B78" s="2"/>
       <c r="G78" s="2">
         <f t="shared" si="2"/>
@@ -3259,8 +3562,12 @@
       <c r="J78" s="9" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K78" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B79" s="2"/>
       <c r="G79" s="2">
         <f t="shared" si="2"/>
@@ -3277,8 +3584,12 @@
       <c r="J79" s="9" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K79" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B80" s="2"/>
       <c r="G80" s="2">
         <f t="shared" si="2"/>
@@ -3295,8 +3606,12 @@
       <c r="J80" s="9" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K80" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" s="2"/>
       <c r="G81" s="2">
         <f t="shared" si="2"/>
@@ -3313,8 +3628,12 @@
       <c r="J81" s="9" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K81" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" s="2"/>
       <c r="G82" s="2">
         <f t="shared" si="2"/>
@@ -3331,8 +3650,12 @@
       <c r="J82" s="9" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K82" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" s="2"/>
       <c r="G83" s="2">
         <f t="shared" si="2"/>
@@ -3349,8 +3672,12 @@
       <c r="J83" s="9" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K83" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" s="2"/>
       <c r="G84" s="2">
         <f t="shared" si="2"/>
@@ -3367,8 +3694,12 @@
       <c r="J84" s="9" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K84" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B85" s="2"/>
       <c r="G85" s="2">
         <f t="shared" si="2"/>
@@ -3385,8 +3716,12 @@
       <c r="J85" s="9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K85" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B86" s="2"/>
       <c r="G86" s="2">
         <f t="shared" si="2"/>
@@ -3403,8 +3738,12 @@
       <c r="J86" s="9" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K86" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" s="2"/>
       <c r="G87" s="2">
         <f t="shared" si="2"/>
@@ -3421,8 +3760,12 @@
       <c r="J87" s="9" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K87" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" s="2"/>
       <c r="G88" s="2">
         <f t="shared" si="2"/>
@@ -3439,8 +3782,12 @@
       <c r="J88" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K88" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B89" s="2"/>
       <c r="G89" s="2">
         <f t="shared" si="2"/>
@@ -3457,8 +3804,12 @@
       <c r="J89" s="9" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K89" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" s="2"/>
       <c r="G90" s="2">
         <f t="shared" ref="G90:G104" si="3">F90/((E90*617.96)+36.04) * 1000000</f>
@@ -3475,8 +3826,12 @@
       <c r="J90" s="9" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K90" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" s="2"/>
       <c r="G91" s="2">
         <f t="shared" si="3"/>
@@ -3493,8 +3848,12 @@
       <c r="J91" s="9" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K91" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" s="2"/>
       <c r="G92" s="2">
         <f t="shared" si="3"/>
@@ -3511,8 +3870,12 @@
       <c r="J92" s="9" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K92" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B93" s="2"/>
       <c r="G93" s="2">
         <f t="shared" si="3"/>
@@ -3529,8 +3892,12 @@
       <c r="J93" s="9" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K93" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="2"/>
       <c r="G94" s="2">
         <f t="shared" si="3"/>
@@ -3547,8 +3914,12 @@
       <c r="J94" s="9" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K94" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" s="2"/>
       <c r="G95" s="2">
         <f t="shared" si="3"/>
@@ -3565,8 +3936,12 @@
       <c r="J95" s="9" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K95" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B96" s="2"/>
       <c r="G96" s="2">
         <f t="shared" si="3"/>
@@ -3583,8 +3958,12 @@
       <c r="J96" s="9" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K96" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B97" s="2"/>
       <c r="G97" s="2">
         <f t="shared" si="3"/>
@@ -3601,8 +3980,12 @@
       <c r="J97" s="9" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K97" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B98" s="2"/>
       <c r="G98" s="2">
         <f t="shared" si="3"/>
@@ -3619,8 +4002,12 @@
       <c r="J98" s="9" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K98" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B99" s="2"/>
       <c r="G99" s="2">
         <f t="shared" si="3"/>
@@ -3637,8 +4024,12 @@
       <c r="J99" s="9" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K99" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B100" s="2"/>
       <c r="G100" s="2">
         <f t="shared" si="3"/>
@@ -3655,8 +4046,12 @@
       <c r="J100" s="9" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K100" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B101" s="2"/>
       <c r="G101" s="2">
         <f t="shared" si="3"/>
@@ -3673,8 +4068,12 @@
       <c r="J101" s="9" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K101" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B102" s="2"/>
       <c r="G102" s="2">
         <f t="shared" si="3"/>
@@ -3691,8 +4090,12 @@
       <c r="J102" s="9" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K102" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B103" s="2"/>
       <c r="G103" s="2">
         <f t="shared" si="3"/>
@@ -3709,8 +4112,12 @@
       <c r="J103" s="9" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K103" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B104" s="2"/>
       <c r="G104" s="2">
         <f t="shared" si="3"/>
@@ -3727,8 +4134,12 @@
       <c r="J104" s="9" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K104" s="9" t="str">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B105" s="2"/>
       <c r="D105" s="2"/>
       <c r="H105" s="2"/>
@@ -3739,7 +4150,7 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="M6" twoDigitTextYear="1"/>
+    <ignoredError sqref="N6" twoDigitTextYear="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3769,7 +4180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D898479-BFF5-2546-B83B-02B04494078A}">
   <dimension ref="B2:F100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A66" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -5151,8 +5562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF35A37-6984-6748-A6C5-DACECEF70E0B}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
more concise transfer commands
</commit_message>
<xml_diff>
--- a/templates/02-ont-plasmid.xlsx
+++ b/templates/02-ont-plasmid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloas/code/opentrons/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D0816D-A40E-FE4C-801E-CC2D3F6C9742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45078B7E-964F-ED41-8852-7CBD12582762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="1360" windowWidth="27920" windowHeight="15940" xr2:uid="{0E74BB9A-F8B8-AA47-B7C7-EA2C2417D685}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="335">
   <si>
     <t>Plasmid sequencing ONT at BCL - Opentrons template</t>
   </si>
@@ -1061,6 +1061,9 @@
   </si>
   <si>
     <t>final pool volume</t>
+  </si>
+  <si>
+    <t>sample 2</t>
   </si>
 </sst>
 </file>
@@ -1608,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842AFD07-9B34-384A-83A8-BAD898DE59C4}">
   <dimension ref="B1:R105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1743,25 +1746,39 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>218</v>
+      </c>
+      <c r="E9">
+        <v>5000</v>
+      </c>
+      <c r="F9">
+        <v>40</v>
+      </c>
       <c r="G9" s="2">
         <f t="shared" ref="G9:G23" si="0">F9/((E9*617.96)+36.04) * 1000000</f>
-        <v>0</v>
+        <v>12.945670735331316</v>
       </c>
       <c r="H9" s="2" cm="1">
         <f t="array" ref="H9">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;4.5,4.5,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>0</v>
+        <v>1.5449180199999999</v>
       </c>
       <c r="I9" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,4.5-Table1[[#This Row],[ul plasmid]])</f>
-        <v>0</v>
+        <v>2.9550819800000001</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>113</v>
       </c>
       <c r="K9" s="9" t="str">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
-        <v/>
+        <v>A02</v>
       </c>
       <c r="M9" t="s">
         <v>328</v>
@@ -1771,25 +1788,39 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
+        <v>334</v>
+      </c>
+      <c r="D10" t="s">
+        <v>214</v>
+      </c>
+      <c r="E10">
+        <v>2000</v>
+      </c>
+      <c r="F10">
+        <v>45</v>
+      </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>36.409061927477616</v>
       </c>
       <c r="H10" s="2" cm="1">
         <f t="array" ref="H10">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;4.5,4.5,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>0</v>
+        <v>0.54931379555555548</v>
       </c>
       <c r="I10" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,4.5-Table1[[#This Row],[ul plasmid]])</f>
-        <v>0</v>
+        <v>3.9506862044444446</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>114</v>
       </c>
       <c r="K10" s="9" t="str">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
-        <v/>
+        <v>E01</v>
       </c>
       <c r="M10" t="s">
         <v>327</v>
@@ -2117,39 +2148,25 @@
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>218</v>
-      </c>
-      <c r="E25">
-        <v>5000</v>
-      </c>
-      <c r="F25">
-        <v>40</v>
-      </c>
+      <c r="B25" s="2"/>
       <c r="G25" s="2">
         <f t="shared" ref="G25:G38" si="2">F25/((E25*617.96)+36.04) * 1000000</f>
-        <v>12.945670735331316</v>
+        <v>0</v>
       </c>
       <c r="H25" s="2" cm="1">
         <f t="array" ref="H25">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;4.5,4.5,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>1.5449180199999999</v>
+        <v>0</v>
       </c>
       <c r="I25" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,4.5-Table1[[#This Row],[ul plasmid]])</f>
-        <v>2.9550819800000001</v>
+        <v>0</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>129</v>
       </c>
       <c r="K25" s="9" t="str">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
-        <v>A02</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
@@ -5362,71 +5379,71 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="str">
         <f>TEXT(main!B9, "")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>113</v>
       </c>
       <c r="C2" s="9">
         <f>main!H9</f>
-        <v>0</v>
+        <v>1.5449180199999999</v>
       </c>
       <c r="D2" s="8" t="str">
         <f>IF(C2=0, "", "A01")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>113</v>
       </c>
       <c r="F2" s="9">
         <f>main!I9</f>
-        <v>0</v>
+        <v>2.9550819800000001</v>
       </c>
       <c r="G2" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D9,Table2[name],Table2[well],"")</f>
-        <v/>
+        <v>A02</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>113</v>
       </c>
       <c r="I2" s="8">
         <f>IF(C2=0,0,0.5)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="str">
         <f>TEXT(main!B10, "")</f>
-        <v/>
+        <v>B01</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>114</v>
       </c>
       <c r="C3" s="9">
         <f>main!H10</f>
-        <v>0</v>
+        <v>0.54931379555555548</v>
       </c>
       <c r="D3" s="8" t="str">
         <f t="shared" ref="D3:D66" si="0">IF(C3=0, "", "A01")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>114</v>
       </c>
       <c r="F3" s="9">
         <f>main!I10</f>
-        <v>0</v>
+        <v>3.9506862044444446</v>
       </c>
       <c r="G3" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D10,Table2[name],Table2[well],"")</f>
-        <v/>
+        <v>E01</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>114</v>
       </c>
       <c r="I3" s="8">
         <f t="shared" ref="I3:I66" si="1">IF(C3=0,0,0.5)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -5922,36 +5939,36 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="str">
         <f>TEXT(main!B25, "")</f>
-        <v>A01</v>
+        <v/>
       </c>
       <c r="B18" s="8" t="s">
         <v>129</v>
       </c>
       <c r="C18" s="9">
         <f>main!H25</f>
-        <v>1.5449180199999999</v>
+        <v>0</v>
       </c>
       <c r="D18" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>A01</v>
+        <v/>
       </c>
       <c r="E18" s="8" t="s">
         <v>129</v>
       </c>
       <c r="F18" s="9">
         <f>main!I25</f>
-        <v>2.9550819800000001</v>
+        <v>0</v>
       </c>
       <c r="G18" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D25,Table2[name],Table2[well],"")</f>
-        <v>A02</v>
+        <v/>
       </c>
       <c r="H18" s="8" t="s">
         <v>129</v>
       </c>
       <c r="I18" s="8">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>